<commit_message>
Add gerador de xlsx nos trinques (CUIDADO com o xlsx de base)
</commit_message>
<xml_diff>
--- a/Assets/Custom Assets/Others/base.xlsx
+++ b/Assets/Custom Assets/Others/base.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="97" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="96" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Relatório" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,28 +15,105 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Cozinhas Telasul Aço</t>
+  </si>
+  <si>
+    <t>Linha:</t>
+  </si>
+  <si>
+    <t>Mirage</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tampo</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="true"/>
+        <color rgb="00000000"/>
+        <sz val="10"/>
+      </rPr>
+      <t xml:space="preserve">:</t>
+    </r>
+  </si>
+  <si>
+    <t>608 - Marmore Preto</t>
+  </si>
+  <si>
+    <t>REF.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DESCRIÇÃO
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="true"/>
+        <color rgb="00FFFFFF"/>
+        <sz val="9"/>
+      </rPr>
+      <t xml:space="preserve">PORTUGUÊS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MEDIDAS
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="00FFFFFF"/>
+        <sz val="9"/>
+      </rPr>
+      <t xml:space="preserve">(LxAxP)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PESO LÍQ. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="00FFFFFF"/>
+        <sz val="9"/>
+      </rPr>
+      <t xml:space="preserve">(Kg)</t>
+    </r>
+  </si>
+  <si>
+    <t>Paneleiro simples - direito</t>
+  </si>
+  <si>
+    <t>400x1940x290</t>
+  </si>
+  <si>
+    <t>informaçõesmóvel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="0.00" numFmtId="165"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="10">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -58,16 +135,67 @@
       <family val="0"/>
       <sz val="10"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="9"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00000000"/>
+        <bgColor rgb="00003300"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
@@ -75,6 +203,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
@@ -101,8 +236,29 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="7" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="6" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -120,39 +276,77 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+      <selection activeCell="D8" activeCellId="0" pane="topLeft" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.5686274509804"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.29803921568628"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.9372549019608"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.7019607843137"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.85" outlineLevel="0" r="4">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="5">
+      <c r="A5" s="6" t="n">
+        <v>33225</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.511805555555555"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;Amp;C&amp;Amp;uot;Times New Roman,Normaluot;&amp;Amp;12&amp;Amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;Amp;C&amp;Amp;uot;Times New Roman,Normaluot;&amp;Amp;12PÃ¡gina &amp;Amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;Amp;C&amp;Amp;Amp;C&amp;Amp;Amp;uot;Times New Roman,Normaluot;&amp;Amp;Amp;12&amp;Amp;Amp;A&amp;Amp;Amp;C&amp;Amp;Amp;uot;Times New Roman,Normaluot;&amp;Amp;Amp;12PÃ¡gina &amp;Amp;Amp;P&amp;Amp;C&amp;Amp;uot;Times New Roman,Normaluot;&amp;Amp;12Página &amp;Amp;P</oddHeader>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>